<commit_message>
Inclusão das horas extras e correções na leitura
</commit_message>
<xml_diff>
--- a/PesquisaOperacional.Gurobi.Core/Data/input.xlsx
+++ b/PesquisaOperacional.Gurobi.Core/Data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uC249567\Dropbox\UFJF\SI\8º período SI\Pesquisa Operacional\Trabalho final\dcc163-pesquisa-operacional-gurobi\PesquisaOperacional.Gurobi.Core\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B249AA6-7686-4EC7-8E9A-BB025E986648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAE523-927F-498A-B058-83D0400ADD3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <author>FAndre.EXT, Jonatas</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{A8DA4833-711B-4D4A-BC58-E9C76E2E5621}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{A8DA4833-711B-4D4A-BC58-E9C76E2E5621}">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Carga horária segunda</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>TOTAL DE CARGA HORÁRIA DA EQUIPE DISPONÍVEL</t>
+  </si>
+  <si>
+    <t>Hora extra</t>
+  </si>
+  <si>
+    <t>Horas normais</t>
   </si>
 </sst>
 </file>
@@ -203,11 +209,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,524 +510,550 @@
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>25</v>
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="G3" s="1">
+        <v>14</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
         <v>18</v>
       </c>
-      <c r="B8" s="3">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
       <c r="E8">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I8">
-        <v>7</v>
+        <v>0.54</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
       <c r="I9">
-        <v>7</v>
+        <v>0.67</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
       <c r="H11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="J11">
-        <v>8</v>
+        <v>12.05</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
       <c r="G12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>6</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>0.67</v>
       </c>
       <c r="J12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>0.27</v>
       </c>
       <c r="J13">
-        <v>8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3">
-        <v>12.5</v>
+        <v>60</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I14">
-        <v>7</v>
+        <v>0.13</v>
       </c>
       <c r="J14">
-        <v>8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3">
-        <v>18</v>
+        <v>12.5</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H15">
         <v>6</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>0.64</v>
       </c>
       <c r="J15">
-        <v>8</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H16">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I16">
-        <v>7</v>
+        <v>0.45</v>
       </c>
       <c r="J16">
-        <v>8</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3">
-        <v>18.666666666666668</v>
+        <v>12</v>
       </c>
       <c r="C17">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>32</v>
+      </c>
+      <c r="H17">
+        <v>12</v>
+      </c>
+      <c r="I17">
+        <v>0.67</v>
+      </c>
+      <c r="J17">
         <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <v>4</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>6</v>
-      </c>
-      <c r="I17">
-        <v>7</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="3">
-        <v>12.5</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>6</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>0.43</v>
       </c>
       <c r="J18">
-        <v>8</v>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="C19">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>42</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>0.64</v>
+      </c>
+      <c r="J19">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Escrita no arquivo de saída e summaries
</commit_message>
<xml_diff>
--- a/PesquisaOperacional.Gurobi.Core/Data/input.xlsx
+++ b/PesquisaOperacional.Gurobi.Core/Data/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uC249567\Dropbox\UFJF\SI\8º período SI\Pesquisa Operacional\Trabalho final\dcc163-pesquisa-operacional-gurobi\PesquisaOperacional.Gurobi.Core\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u6026969\source\repos\PesquisaOperacional.Gurobi.Core\PesquisaOperacional.Gurobi.Core\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAE523-927F-498A-B058-83D0400ADD3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A10F53-6D73-4C8E-A6FC-9A9632D56509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,22 +558,22 @@
         <v>31</v>
       </c>
       <c r="B3" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -584,22 +584,22 @@
         <v>30</v>
       </c>
       <c r="B4" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>18</v>

</xml_diff>